<commit_message>
remove mobile number those who i am added
</commit_message>
<xml_diff>
--- a/dataBaseStructure.xlsx
+++ b/dataBaseStructure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Database structure\DataBase-Structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D71C5E1-0D31-443C-BB44-8BBC200C8B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BDE433-AE55-4EEB-B25B-095A94A7D596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="35">
   <si>
     <t>Data types</t>
   </si>
@@ -135,12 +135,6 @@
   </si>
   <si>
     <t>email</t>
-  </si>
-  <si>
-    <t>mobile</t>
-  </si>
-  <si>
-    <t>int</t>
   </si>
 </sst>
 </file>
@@ -538,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,14 +570,6 @@
       </c>
       <c r="B3" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change Account to AccountName
</commit_message>
<xml_diff>
--- a/dataBaseStructure.xlsx
+++ b/dataBaseStructure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Database structure\DataBase-Structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BDE433-AE55-4EEB-B25B-095A94A7D596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C806F07B-58E9-4365-A108-2D340E20D8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dishCategory" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,6 @@
     <t>categoryId</t>
   </si>
   <si>
-    <t>account</t>
-  </si>
-  <si>
     <t>accountNumber</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>email</t>
+  </si>
+  <si>
+    <t>accountName</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,7 +824,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -832,7 +832,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -840,7 +840,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -848,7 +848,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -906,7 +906,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -914,7 +914,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Added User Config Fields
</commit_message>
<xml_diff>
--- a/dataBaseStructure.xlsx
+++ b/dataBaseStructure.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Database structure\DataBase-Structure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DataBaseStructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C806F07B-58E9-4365-A108-2D340E20D8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="dishCategory" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,9 @@
     <sheet name="clientCategory" sheetId="4" r:id="rId3"/>
     <sheet name="clientBankDetail" sheetId="5" r:id="rId4"/>
     <sheet name="userConfig" sheetId="6" r:id="rId5"/>
-    <sheet name="Client" sheetId="3" r:id="rId6"/>
+    <sheet name="City" sheetId="7" r:id="rId6"/>
+    <sheet name="Client" sheetId="3" r:id="rId7"/>
+    <sheet name="State" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="38">
   <si>
     <t>Data types</t>
   </si>
@@ -136,12 +137,21 @@
   <si>
     <t>accountName</t>
   </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,16 +164,30 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor theme="8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -171,15 +195,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -198,72 +259,72 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C4" totalsRowShown="0">
+  <autoFilter ref="A1:C4"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Property name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Data types"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Default values"/>
+    <tableColumn id="1" name="Property name"/>
+    <tableColumn id="2" name="Data types"/>
+    <tableColumn id="3" name="Default values"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:C17" totalsRowShown="0">
-  <autoFilter ref="A1:C17" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:C17" totalsRowShown="0">
+  <autoFilter ref="A1:C17"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Property name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Data types"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Default values"/>
+    <tableColumn id="1" name="Property name"/>
+    <tableColumn id="2" name="Data types"/>
+    <tableColumn id="3" name="Default values"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table15" displayName="Table15" ref="A1:C3" totalsRowShown="0">
-  <autoFilter ref="A1:C3" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:C3" totalsRowShown="0">
+  <autoFilter ref="A1:C3"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Property name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Data types"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Default values"/>
+    <tableColumn id="1" name="Property name"/>
+    <tableColumn id="2" name="Data types"/>
+    <tableColumn id="3" name="Default values"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table16" displayName="Table16" ref="A1:C7" totalsRowShown="0">
-  <autoFilter ref="A1:C7" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="A1:C7" totalsRowShown="0">
+  <autoFilter ref="A1:C7"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Property name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Data types"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Default values"/>
+    <tableColumn id="1" name="Property name"/>
+    <tableColumn id="2" name="Data types"/>
+    <tableColumn id="3" name="Default values"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table17" displayName="Table17" ref="A1:C5" totalsRowShown="0">
-  <autoFilter ref="A1:C5" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table17" displayName="Table17" ref="A1:C8" totalsRowShown="0">
+  <autoFilter ref="A1:C8"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Property name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Data types"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Default values"/>
+    <tableColumn id="1" name="Property name"/>
+    <tableColumn id="2" name="Data types"/>
+    <tableColumn id="3" name="Default values"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table14" displayName="Table14" ref="A1:C9" totalsRowShown="0">
-  <autoFilter ref="A1:C9" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:C9" totalsRowShown="0">
+  <autoFilter ref="A1:C9"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Property name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Data types"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Default values"/>
+    <tableColumn id="1" name="Property name"/>
+    <tableColumn id="2" name="Data types"/>
+    <tableColumn id="3" name="Default values"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -531,7 +592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -581,7 +642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -739,7 +800,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -789,10 +850,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -871,11 +932,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,6 +989,30 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -937,7 +1022,51 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1021,4 +1150,48 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Re-defined Admin and his bank details
</commit_message>
<xml_diff>
--- a/dataBaseStructure.xlsx
+++ b/dataBaseStructure.xlsx
@@ -9,17 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="dishCategory" sheetId="1" r:id="rId1"/>
     <sheet name="dish" sheetId="2" r:id="rId2"/>
-    <sheet name="clientCategory" sheetId="4" r:id="rId3"/>
-    <sheet name="clientBankDetail" sheetId="5" r:id="rId4"/>
-    <sheet name="userConfig" sheetId="6" r:id="rId5"/>
-    <sheet name="City" sheetId="7" r:id="rId6"/>
-    <sheet name="Client" sheetId="3" r:id="rId7"/>
-    <sheet name="State" sheetId="8" r:id="rId8"/>
+    <sheet name="BankDetails" sheetId="5" r:id="rId3"/>
+    <sheet name="userConfig" sheetId="6" r:id="rId4"/>
+    <sheet name="City" sheetId="7" r:id="rId5"/>
+    <sheet name="Admin" sheetId="3" r:id="rId6"/>
+    <sheet name="State" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="46">
   <si>
     <t>Data types</t>
   </si>
@@ -102,9 +101,6 @@
     <t>cookingTime</t>
   </si>
   <si>
-    <t>business</t>
-  </si>
-  <si>
     <t>address</t>
   </si>
   <si>
@@ -114,12 +110,6 @@
     <t>foodclass</t>
   </si>
   <si>
-    <t>categoryName</t>
-  </si>
-  <si>
-    <t>categoryId</t>
-  </si>
-  <si>
     <t>accountNumber</t>
   </si>
   <si>
@@ -145,6 +135,39 @@
   </si>
   <si>
     <t>pincode</t>
+  </si>
+  <si>
+    <t>UPICodeImg</t>
+  </si>
+  <si>
+    <t>UPICodeNumber</t>
+  </si>
+  <si>
+    <t>businessName</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>foodLincNum</t>
+  </si>
+  <si>
+    <t>bankDetails</t>
+  </si>
+  <si>
+    <t>BankDetails</t>
+  </si>
+  <si>
+    <t>restaurentLogo</t>
+  </si>
+  <si>
+    <t>restaurentSeal</t>
+  </si>
+  <si>
+    <t>signature</t>
+  </si>
+  <si>
+    <t>termAndCondition</t>
   </si>
 </sst>
 </file>
@@ -283,8 +306,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:C3" totalsRowShown="0">
-  <autoFilter ref="A1:C3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="A1:C8" totalsRowShown="0">
+  <autoFilter ref="A1:C8"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Property name"/>
     <tableColumn id="2" name="Data types"/>
@@ -295,18 +318,6 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="A1:C7" totalsRowShown="0">
-  <autoFilter ref="A1:C7"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Property name"/>
-    <tableColumn id="2" name="Data types"/>
-    <tableColumn id="3" name="Default values"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table17" displayName="Table17" ref="A1:C8" totalsRowShown="0">
   <autoFilter ref="A1:C8"/>
   <tableColumns count="3">
@@ -318,9 +329,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:C9" totalsRowShown="0">
-  <autoFilter ref="A1:C9"/>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:C15" totalsRowShown="0">
+  <autoFilter ref="A1:C15"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Property name"/>
     <tableColumn id="2" name="Data types"/>
@@ -801,10 +812,92 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,10 +928,50 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -849,17 +982,61 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -885,7 +1062,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -893,23 +1070,23 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -920,6 +1097,59 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
         <v>20</v>
       </c>
     </row>
@@ -931,232 +1161,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="7"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>